<commit_message>
Pressure loss calculations for propellant lines + update to pipe couplings docs
</commit_message>
<xml_diff>
--- a/Piping/Propellant Piping/Piping (prop) requirements.xlsx
+++ b/Piping/Propellant Piping/Piping (prop) requirements.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Piping/Propellant Piping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0680463-1567-454C-9725-704B9B8CE32B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E491AB2-F1F6-414E-ADC5-97EFBB436C89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{35CE8334-D947-1140-A1D1-031EDAB2315E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{35CE8334-D947-1140-A1D1-031EDAB2315E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Docs" sheetId="1" r:id="rId1"/>
+    <sheet name="Design" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,20 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Propellant Piping</t>
   </si>
   <si>
-    <t>Inlet Pipes</t>
-  </si>
-  <si>
-    <t>Pre-Pump Pipes</t>
-  </si>
-  <si>
-    <t>Post-Pump Pipes</t>
-  </si>
-  <si>
     <t>Mdot = Density * Flow Rate * Cross Sectional Area</t>
   </si>
   <si>
@@ -55,13 +47,34 @@
   </si>
   <si>
     <t>Pipe Diameter = sqrt(4) * Flow Rate / pi * velocity</t>
+  </si>
+  <si>
+    <t>Cals</t>
+  </si>
+  <si>
+    <t>LOX Density</t>
+  </si>
+  <si>
+    <t>Ethanol Density</t>
+  </si>
+  <si>
+    <t>Flow Rate</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Pi</t>
+  </si>
+  <si>
+    <t>kgm^3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -78,8 +91,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="16"/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -106,15 +133,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,42 +459,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2BB5F7-F5F1-F74F-8942-B9C33DB92B77}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="4" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="5" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -472,12 +523,33 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+    <row r="9" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -485,46 +557,108 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="13" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>9</v>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="17" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>3.1141592653589698</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A12:C12"/>
+  <mergeCells count="3">
     <mergeCell ref="F4:K4"/>
     <mergeCell ref="F8:K8"/>
     <mergeCell ref="F12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E3F3EF-8FD7-E649-A7FB-461CF53584D1}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1141</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>789</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>